<commit_message>
Test Data sheet added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -58,37 +58,37 @@
     <t>Cart page</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Suite1</t>
+  </si>
+  <si>
+    <t>Checkout Page</t>
+  </si>
+  <si>
+    <t>Suite2</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Suite3</t>
+  </si>
+  <si>
+    <t>Order Summary Page</t>
+  </si>
+  <si>
+    <t>Suite4</t>
+  </si>
+  <si>
+    <t>URL Tests</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Suite1</t>
-  </si>
-  <si>
-    <t>Checkout Page</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Suite2</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>Suite3</t>
-  </si>
-  <si>
-    <t>Order Summary Page</t>
-  </si>
-  <si>
-    <t>Suite4</t>
-  </si>
-  <si>
-    <t>URL Tests</t>
   </si>
   <si>
     <t>REST</t>
@@ -864,10 +864,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -936,7 +936,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -944,6 +944,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1001,13 +1008,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1047,6 +1047,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1069,15 +1070,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1111,19 +1111,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1141,7 +1135,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1153,25 +1153,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1184,6 +1172,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1213,7 +1213,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1225,7 +1231,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1237,7 +1261,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1249,25 +1273,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1279,19 +1285,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1409,15 +1409,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1432,23 +1423,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -1457,118 +1457,118 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="E3" s="25">
         <f>IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:5">
@@ -2118,13 +2118,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="25">
         <f>IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
@@ -2133,16 +2133,16 @@
     </row>
     <row r="5" ht="15.75" spans="1:5">
       <c r="A5" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="25">
         <f>IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
@@ -2151,16 +2151,16 @@
     </row>
     <row r="6" ht="15.75" spans="1:5">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="25">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="7" ht="15.75" spans="1:5">
       <c r="A7" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>19</v>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="E8" s="25">
         <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:5">
@@ -2329,7 +2329,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B21" s="29">
         <f>SUM(E3:E15)</f>
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2386,7 +2386,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -2397,7 +2397,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -2408,7 +2408,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -2483,7 +2483,7 @@
         <v>263</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>264</v>
@@ -2497,7 +2497,7 @@
         <v>265</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>266</v>
@@ -2511,7 +2511,7 @@
         <v>267</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>268</v>
@@ -2562,7 +2562,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>48</v>
@@ -2576,7 +2576,7 @@
         <v>50</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>51</v>
@@ -2590,7 +2590,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>53</v>
@@ -2604,7 +2604,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>55</v>
@@ -2618,7 +2618,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>57</v>
@@ -2632,7 +2632,7 @@
         <v>59</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>60</v>
@@ -2646,7 +2646,7 @@
         <v>61</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>62</v>
@@ -2660,7 +2660,7 @@
         <v>63</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>64</v>
@@ -2674,7 +2674,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>66</v>
@@ -2689,7 +2689,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>68</v>
@@ -2703,7 +2703,7 @@
         <v>69</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>70</v>
@@ -2717,7 +2717,7 @@
         <v>71</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>72</v>
@@ -2731,7 +2731,7 @@
         <v>73</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>74</v>
@@ -2745,7 +2745,7 @@
         <v>75</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>76</v>
@@ -2759,7 +2759,7 @@
         <v>77</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>78</v>
@@ -2773,7 +2773,7 @@
         <v>79</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>80</v>
@@ -2787,7 +2787,7 @@
         <v>81</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>82</v>
@@ -2835,7 +2835,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>84</v>
@@ -2846,7 +2846,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>86</v>
@@ -2857,7 +2857,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>88</v>
@@ -2868,7 +2868,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>90</v>
@@ -2879,7 +2879,7 @@
         <v>91</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>92</v>
@@ -2890,7 +2890,7 @@
         <v>93</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>94</v>
@@ -2901,7 +2901,7 @@
         <v>95</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>96</v>
@@ -2912,7 +2912,7 @@
         <v>97</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>98</v>
@@ -2923,7 +2923,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>100</v>
@@ -2934,7 +2934,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>102</v>
@@ -2945,7 +2945,7 @@
         <v>103</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>104</v>
@@ -2956,7 +2956,7 @@
         <v>105</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>104</v>
@@ -2967,7 +2967,7 @@
         <v>106</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>107</v>
@@ -2978,7 +2978,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>109</v>
@@ -2989,7 +2989,7 @@
         <v>110</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>111</v>
@@ -3000,7 +3000,7 @@
         <v>112</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>113</v>
@@ -3011,7 +3011,7 @@
         <v>114</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>115</v>
@@ -3022,7 +3022,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>117</v>
@@ -3033,7 +3033,7 @@
         <v>118</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>119</v>
@@ -3082,7 +3082,7 @@
         <v>120</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>121</v>
@@ -3096,7 +3096,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>123</v>
@@ -3110,7 +3110,7 @@
         <v>124</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>125</v>
@@ -3124,7 +3124,7 @@
         <v>126</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>127</v>
@@ -3138,7 +3138,7 @@
         <v>128</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>129</v>
@@ -3152,7 +3152,7 @@
         <v>130</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>131</v>
@@ -3166,7 +3166,7 @@
         <v>132</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>133</v>
@@ -3180,7 +3180,7 @@
         <v>134</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>135</v>
@@ -3194,7 +3194,7 @@
         <v>136</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>137</v>
@@ -3208,7 +3208,7 @@
         <v>138</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>139</v>
@@ -3222,7 +3222,7 @@
         <v>140</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>141</v>
@@ -3236,7 +3236,7 @@
         <v>142</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>143</v>
@@ -3250,7 +3250,7 @@
         <v>144</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>145</v>
@@ -3264,7 +3264,7 @@
         <v>146</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>147</v>
@@ -3278,7 +3278,7 @@
         <v>148</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>149</v>
@@ -3292,7 +3292,7 @@
         <v>150</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>151</v>
@@ -3306,7 +3306,7 @@
         <v>152</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>153</v>
@@ -3320,7 +3320,7 @@
         <v>154</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>155</v>
@@ -3334,7 +3334,7 @@
         <v>156</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>157</v>
@@ -3348,7 +3348,7 @@
         <v>158</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>159</v>
@@ -3362,7 +3362,7 @@
         <v>160</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>161</v>
@@ -3376,7 +3376,7 @@
         <v>162</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>163</v>
@@ -3390,7 +3390,7 @@
         <v>164</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>165</v>
@@ -3404,7 +3404,7 @@
         <v>166</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>167</v>
@@ -3418,7 +3418,7 @@
         <v>169</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>170</v>
@@ -3471,7 +3471,7 @@
         <v>171</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>172</v>
@@ -3485,7 +3485,7 @@
         <v>173</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>174</v>
@@ -3499,7 +3499,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>176</v>
@@ -3513,7 +3513,7 @@
         <v>177</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>178</v>
@@ -3527,7 +3527,7 @@
         <v>179</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>180</v>
@@ -3541,7 +3541,7 @@
         <v>181</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>182</v>
@@ -3555,7 +3555,7 @@
         <v>183</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>184</v>
@@ -3569,7 +3569,7 @@
         <v>185</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>186</v>
@@ -3624,7 +3624,7 @@
         <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>188</v>
@@ -3679,7 +3679,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>190</v>
@@ -3693,7 +3693,7 @@
         <v>191</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>192</v>
@@ -3707,7 +3707,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>194</v>
@@ -3721,7 +3721,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>196</v>
@@ -3735,7 +3735,7 @@
         <v>197</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>198</v>
@@ -3749,7 +3749,7 @@
         <v>199</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>200</v>
@@ -3763,7 +3763,7 @@
         <v>201</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>202</v>
@@ -3777,7 +3777,7 @@
         <v>203</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>204</v>
@@ -3791,7 +3791,7 @@
         <v>205</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>206</v>
@@ -3805,7 +3805,7 @@
         <v>207</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>208</v>
@@ -3819,7 +3819,7 @@
         <v>209</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>210</v>
@@ -3833,7 +3833,7 @@
         <v>211</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>212</v>
@@ -3847,7 +3847,7 @@
         <v>213</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>214</v>
@@ -3861,7 +3861,7 @@
         <v>215</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>216</v>
@@ -3875,7 +3875,7 @@
         <v>217</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>218</v>
@@ -3889,7 +3889,7 @@
         <v>219</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>220</v>
@@ -3903,7 +3903,7 @@
         <v>221</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>222</v>
@@ -3917,7 +3917,7 @@
         <v>223</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>224</v>
@@ -3931,7 +3931,7 @@
         <v>225</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>226</v>
@@ -3945,7 +3945,7 @@
         <v>227</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>228</v>
@@ -3959,7 +3959,7 @@
         <v>229</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>230</v>
@@ -3973,7 +3973,7 @@
         <v>231</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>232</v>
@@ -3987,7 +3987,7 @@
         <v>233</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>234</v>
@@ -4001,7 +4001,7 @@
         <v>235</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>236</v>
@@ -4015,7 +4015,7 @@
         <v>237</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>238</v>
@@ -4029,7 +4029,7 @@
         <v>239</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>240</v>
@@ -4043,7 +4043,7 @@
         <v>241</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>242</v>
@@ -4057,7 +4057,7 @@
         <v>243</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>244</v>
@@ -4071,7 +4071,7 @@
         <v>245</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>246</v>
@@ -4085,7 +4085,7 @@
         <v>247</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>248</v>
@@ -4099,7 +4099,7 @@
         <v>249</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>250</v>
@@ -4155,7 +4155,7 @@
         <v>251</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>252</v>
@@ -4169,7 +4169,7 @@
         <v>253</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>254</v>
@@ -4183,7 +4183,7 @@
         <v>255</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>256</v>
@@ -4240,7 +4240,7 @@
         <v>257</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>258</v>
@@ -4254,7 +4254,7 @@
         <v>259</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>260</v>
@@ -4268,7 +4268,7 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>262</v>

</xml_diff>

<commit_message>
Code updated for Build
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -58,18 +58,21 @@
     <t>Cart page</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Suite1</t>
+  </si>
+  <si>
+    <t>Checkout Page</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Suite1</t>
-  </si>
-  <si>
-    <t>Checkout Page</t>
-  </si>
-  <si>
     <t>Suite2</t>
   </si>
   <si>
@@ -86,9 +89,6 @@
   </si>
   <si>
     <t>URL Tests</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>REST</t>
@@ -866,8 +866,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -936,7 +936,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -944,13 +944,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1008,6 +1001,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1047,14 +1047,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -1078,6 +1070,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1111,7 +1111,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1135,7 +1135,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1159,7 +1159,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1177,7 +1177,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1213,31 +1213,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1255,13 +1231,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1273,13 +1255,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,6 +1274,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1437,18 +1437,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -1457,118 +1457,118 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2054,7 +2054,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="E3" s="25">
         <f>IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:5">
@@ -2118,13 +2118,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="25">
         <f>IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
@@ -2133,16 +2133,16 @@
     </row>
     <row r="5" ht="15.75" spans="1:5">
       <c r="A5" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="25">
         <f>IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
@@ -2151,16 +2151,16 @@
     </row>
     <row r="6" ht="15.75" spans="1:5">
       <c r="A6" s="24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="25">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="7" ht="15.75" spans="1:5">
       <c r="A7" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>19</v>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="E7" s="25">
         <f>IF(B7="Y",COUNTIF(Suite5!B2:B51,"Y"),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:5">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="E8" s="25">
         <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:5">
@@ -2241,7 +2241,7 @@
       <c r="A11" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -2329,7 +2329,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B21" s="29">
         <f>SUM(E3:E15)</f>
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2386,7 +2386,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -2397,7 +2397,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -2408,7 +2408,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -2483,7 +2483,7 @@
         <v>263</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>264</v>
@@ -2497,7 +2497,7 @@
         <v>265</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>266</v>
@@ -2511,7 +2511,7 @@
         <v>267</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>268</v>
@@ -2562,7 +2562,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>48</v>
@@ -2576,7 +2576,7 @@
         <v>50</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>51</v>
@@ -2590,7 +2590,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>53</v>
@@ -2604,7 +2604,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>55</v>
@@ -2618,7 +2618,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>57</v>
@@ -2632,7 +2632,7 @@
         <v>59</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>60</v>
@@ -2646,7 +2646,7 @@
         <v>61</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>62</v>
@@ -2660,7 +2660,7 @@
         <v>63</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>64</v>
@@ -2674,7 +2674,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>66</v>
@@ -2689,7 +2689,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>68</v>
@@ -2703,7 +2703,7 @@
         <v>69</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>70</v>
@@ -2717,7 +2717,7 @@
         <v>71</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>72</v>
@@ -2731,7 +2731,7 @@
         <v>73</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>74</v>
@@ -2745,7 +2745,7 @@
         <v>75</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>76</v>
@@ -2759,7 +2759,7 @@
         <v>77</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>78</v>
@@ -2773,7 +2773,7 @@
         <v>79</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>80</v>
@@ -2787,7 +2787,7 @@
         <v>81</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>82</v>
@@ -2835,7 +2835,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>84</v>
@@ -2846,7 +2846,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>86</v>
@@ -2857,7 +2857,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>88</v>
@@ -2868,7 +2868,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>90</v>
@@ -2879,7 +2879,7 @@
         <v>91</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>92</v>
@@ -2890,7 +2890,7 @@
         <v>93</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>94</v>
@@ -2901,7 +2901,7 @@
         <v>95</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>96</v>
@@ -2912,7 +2912,7 @@
         <v>97</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>98</v>
@@ -2923,7 +2923,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>100</v>
@@ -2934,7 +2934,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>102</v>
@@ -2945,7 +2945,7 @@
         <v>103</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>104</v>
@@ -2956,7 +2956,7 @@
         <v>105</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>104</v>
@@ -2967,7 +2967,7 @@
         <v>106</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>107</v>
@@ -2978,7 +2978,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>109</v>
@@ -2989,7 +2989,7 @@
         <v>110</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>111</v>
@@ -3000,7 +3000,7 @@
         <v>112</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>113</v>
@@ -3011,7 +3011,7 @@
         <v>114</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>115</v>
@@ -3022,7 +3022,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>117</v>
@@ -3033,7 +3033,7 @@
         <v>118</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>119</v>
@@ -3082,7 +3082,7 @@
         <v>120</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>121</v>
@@ -3096,7 +3096,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>123</v>
@@ -3110,7 +3110,7 @@
         <v>124</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>125</v>
@@ -3124,7 +3124,7 @@
         <v>126</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>127</v>
@@ -3138,7 +3138,7 @@
         <v>128</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>129</v>
@@ -3152,7 +3152,7 @@
         <v>130</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>131</v>
@@ -3166,7 +3166,7 @@
         <v>132</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>133</v>
@@ -3180,7 +3180,7 @@
         <v>134</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>135</v>
@@ -3194,7 +3194,7 @@
         <v>136</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>137</v>
@@ -3208,7 +3208,7 @@
         <v>138</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>139</v>
@@ -3222,7 +3222,7 @@
         <v>140</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>141</v>
@@ -3236,7 +3236,7 @@
         <v>142</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>143</v>
@@ -3250,7 +3250,7 @@
         <v>144</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>145</v>
@@ -3264,7 +3264,7 @@
         <v>146</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>147</v>
@@ -3278,7 +3278,7 @@
         <v>148</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>149</v>
@@ -3292,7 +3292,7 @@
         <v>150</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>151</v>
@@ -3306,7 +3306,7 @@
         <v>152</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>153</v>
@@ -3320,7 +3320,7 @@
         <v>154</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>155</v>
@@ -3334,7 +3334,7 @@
         <v>156</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>157</v>
@@ -3348,7 +3348,7 @@
         <v>158</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>159</v>
@@ -3362,7 +3362,7 @@
         <v>160</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>161</v>
@@ -3376,7 +3376,7 @@
         <v>162</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>163</v>
@@ -3390,7 +3390,7 @@
         <v>164</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>165</v>
@@ -3404,7 +3404,7 @@
         <v>166</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>167</v>
@@ -3418,7 +3418,7 @@
         <v>169</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>170</v>
@@ -3471,7 +3471,7 @@
         <v>171</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>172</v>
@@ -3485,7 +3485,7 @@
         <v>173</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>174</v>
@@ -3499,7 +3499,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>176</v>
@@ -3513,7 +3513,7 @@
         <v>177</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>178</v>
@@ -3527,7 +3527,7 @@
         <v>179</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>180</v>
@@ -3541,7 +3541,7 @@
         <v>181</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>182</v>
@@ -3555,7 +3555,7 @@
         <v>183</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>184</v>
@@ -3569,7 +3569,7 @@
         <v>185</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>186</v>
@@ -3624,7 +3624,7 @@
         <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>188</v>
@@ -3679,7 +3679,7 @@
         <v>189</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>190</v>
@@ -3693,7 +3693,7 @@
         <v>191</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>192</v>
@@ -3707,7 +3707,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>194</v>
@@ -3721,7 +3721,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>196</v>
@@ -3735,7 +3735,7 @@
         <v>197</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>198</v>
@@ -3749,7 +3749,7 @@
         <v>199</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>200</v>
@@ -3763,7 +3763,7 @@
         <v>201</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>202</v>
@@ -3777,7 +3777,7 @@
         <v>203</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>204</v>
@@ -3791,7 +3791,7 @@
         <v>205</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>206</v>
@@ -3805,7 +3805,7 @@
         <v>207</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>208</v>
@@ -3819,7 +3819,7 @@
         <v>209</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>210</v>
@@ -3833,7 +3833,7 @@
         <v>211</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>212</v>
@@ -3847,7 +3847,7 @@
         <v>213</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>214</v>
@@ -3861,7 +3861,7 @@
         <v>215</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>216</v>
@@ -3875,7 +3875,7 @@
         <v>217</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>218</v>
@@ -3889,7 +3889,7 @@
         <v>219</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>220</v>
@@ -3903,7 +3903,7 @@
         <v>221</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>222</v>
@@ -3917,7 +3917,7 @@
         <v>223</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>224</v>
@@ -3931,7 +3931,7 @@
         <v>225</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>226</v>
@@ -3945,7 +3945,7 @@
         <v>227</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>228</v>
@@ -3959,7 +3959,7 @@
         <v>229</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>230</v>
@@ -3973,7 +3973,7 @@
         <v>231</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>232</v>
@@ -3987,7 +3987,7 @@
         <v>233</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>234</v>
@@ -4001,7 +4001,7 @@
         <v>235</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>236</v>
@@ -4015,7 +4015,7 @@
         <v>237</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>238</v>
@@ -4029,7 +4029,7 @@
         <v>239</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>240</v>
@@ -4043,7 +4043,7 @@
         <v>241</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>242</v>
@@ -4057,7 +4057,7 @@
         <v>243</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>244</v>
@@ -4071,7 +4071,7 @@
         <v>245</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>246</v>
@@ -4085,7 +4085,7 @@
         <v>247</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>248</v>
@@ -4099,7 +4099,7 @@
         <v>249</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>250</v>
@@ -4155,7 +4155,7 @@
         <v>251</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>252</v>
@@ -4169,7 +4169,7 @@
         <v>253</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>254</v>
@@ -4183,7 +4183,7 @@
         <v>255</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>256</v>
@@ -4240,7 +4240,7 @@
         <v>257</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>258</v>
@@ -4254,7 +4254,7 @@
         <v>259</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>260</v>
@@ -4268,7 +4268,7 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>262</v>

</xml_diff>

<commit_message>
Checkout test scripts added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="987"/>
+    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="987" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,12 @@
     <definedName name="Suite5">#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:G10"/>
+  <oleSize ref="A19:G28"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -392,6 +392,48 @@
   </si>
   <si>
     <t>Order Summary : Place Order : Ensure  that when user click on 'Place Order'  it has to navigate to  "Payment page".</t>
+  </si>
+  <si>
+    <t>IGP_TC_178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add New Address:Ensure that logged-in user is able to see add new address option. </t>
+  </si>
+  <si>
+    <t>IGP_TC_179</t>
+  </si>
+  <si>
+    <t>Sign Up:Ensure that a new user is able to sign in.</t>
+  </si>
+  <si>
+    <t>IGP_TC_180</t>
+  </si>
+  <si>
+    <t>Login through Facebook: Ensure that a new user is able to login through Facebook</t>
+  </si>
+  <si>
+    <t>IGP_TC_181</t>
+  </si>
+  <si>
+    <t>Login through Google+: Ensure that a new user is able to login through Google+</t>
+  </si>
+  <si>
+    <t>IGP_TC_182</t>
+  </si>
+  <si>
+    <t>Forgot Password: Ensure that user should be able to reset password</t>
+  </si>
+  <si>
+    <t>IGP_TC_183</t>
+  </si>
+  <si>
+    <t>Remove Product from link:Ensure that user able to remove the  product from Link.</t>
+  </si>
+  <si>
+    <t>IGP_TC_184</t>
+  </si>
+  <si>
+    <t>Delivery is not supported in USA:Ensure that the user experiences a warning message when delivery is not supported for India.</t>
   </si>
   <si>
     <t>IGP_TC_195</t>
@@ -864,9 +906,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
@@ -935,50 +977,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -990,6 +995,22 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1008,9 +1029,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1024,26 +1089,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1054,30 +1103,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1111,19 +1153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1141,7 +1171,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1153,13 +1261,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1171,7 +1303,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1183,115 +1315,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1335,6 +1377,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1350,31 +1410,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1394,21 +1455,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1418,17 +1464,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1437,138 +1479,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2053,7 +2095,7 @@
   <sheetPr/>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2127,7 +2169,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="25">
-        <f>IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
+        <f>IF(B4="Y",COUNTIF(Suite2!B2:B49,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2480,13 +2522,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -2494,13 +2536,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -2508,13 +2550,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -2803,10 +2845,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3038,6 +3080,93 @@
       <c r="C20" s="15" t="s">
         <v>119</v>
       </c>
+    </row>
+    <row r="21" ht="30" spans="1:3">
+      <c r="A21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" ht="30" spans="1:3">
+      <c r="A22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" ht="30" spans="1:3">
+      <c r="A23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" ht="30" spans="1:3">
+      <c r="A24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" ht="30" spans="1:3">
+      <c r="A25" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" ht="30" spans="1:3">
+      <c r="A26" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" ht="45" spans="1:3">
+      <c r="A27" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
@@ -3079,13 +3208,13 @@
     </row>
     <row r="2" ht="45" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -3093,13 +3222,13 @@
     </row>
     <row r="3" ht="30" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -3107,13 +3236,13 @@
     </row>
     <row r="4" ht="30" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -3121,13 +3250,13 @@
     </row>
     <row r="5" ht="45" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>49</v>
@@ -3135,13 +3264,13 @@
     </row>
     <row r="6" ht="45" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
@@ -3149,13 +3278,13 @@
     </row>
     <row r="7" ht="45" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>49</v>
@@ -3163,13 +3292,13 @@
     </row>
     <row r="8" ht="45" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>49</v>
@@ -3177,13 +3306,13 @@
     </row>
     <row r="9" ht="30" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>49</v>
@@ -3191,13 +3320,13 @@
     </row>
     <row r="10" ht="45" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>49</v>
@@ -3205,13 +3334,13 @@
     </row>
     <row r="11" ht="45" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>49</v>
@@ -3219,13 +3348,13 @@
     </row>
     <row r="12" ht="60" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>49</v>
@@ -3233,13 +3362,13 @@
     </row>
     <row r="13" ht="30" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
@@ -3247,13 +3376,13 @@
     </row>
     <row r="14" ht="30" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
@@ -3261,13 +3390,13 @@
     </row>
     <row r="15" ht="30" spans="1:4">
       <c r="A15" s="5" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>49</v>
@@ -3275,13 +3404,13 @@
     </row>
     <row r="16" ht="30" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>49</v>
@@ -3289,13 +3418,13 @@
     </row>
     <row r="17" ht="30" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
@@ -3303,13 +3432,13 @@
     </row>
     <row r="18" ht="30" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>49</v>
@@ -3317,13 +3446,13 @@
     </row>
     <row r="19" ht="45" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>49</v>
@@ -3331,13 +3460,13 @@
     </row>
     <row r="20" ht="30" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>49</v>
@@ -3345,13 +3474,13 @@
     </row>
     <row r="21" ht="30" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>49</v>
@@ -3359,13 +3488,13 @@
     </row>
     <row r="22" ht="30" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>49</v>
@@ -3373,13 +3502,13 @@
     </row>
     <row r="23" ht="30" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>49</v>
@@ -3387,13 +3516,13 @@
     </row>
     <row r="24" ht="30" spans="1:4">
       <c r="A24" s="5" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>49</v>
@@ -3401,27 +3530,27 @@
     </row>
     <row r="25" ht="30" spans="1:4">
       <c r="A25" s="5" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" ht="45" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>49</v>
@@ -3468,13 +3597,13 @@
     </row>
     <row r="2" ht="45" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>49</v>
@@ -3482,13 +3611,13 @@
     </row>
     <row r="3" ht="45" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>49</v>
@@ -3496,13 +3625,13 @@
     </row>
     <row r="4" ht="30" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>49</v>
@@ -3510,13 +3639,13 @@
     </row>
     <row r="5" ht="30" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>49</v>
@@ -3524,13 +3653,13 @@
     </row>
     <row r="6" ht="30" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>49</v>
@@ -3538,13 +3667,13 @@
     </row>
     <row r="7" ht="30" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -3552,13 +3681,13 @@
     </row>
     <row r="8" ht="30" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
         <v>49</v>
@@ -3566,13 +3695,13 @@
     </row>
     <row r="9" ht="30" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
@@ -3621,13 +3750,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
         <v>49</v>
@@ -3676,13 +3805,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="45" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>49</v>
@@ -3690,13 +3819,13 @@
     </row>
     <row r="3" ht="45" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>49</v>
@@ -3704,13 +3833,13 @@
     </row>
     <row r="4" ht="45" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>49</v>
@@ -3718,13 +3847,13 @@
     </row>
     <row r="5" ht="60" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>49</v>
@@ -3732,13 +3861,13 @@
     </row>
     <row r="6" ht="45" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
@@ -3746,13 +3875,13 @@
     </row>
     <row r="7" ht="45" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>49</v>
@@ -3760,13 +3889,13 @@
     </row>
     <row r="8" ht="30" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>49</v>
@@ -3774,13 +3903,13 @@
     </row>
     <row r="9" ht="45" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>49</v>
@@ -3788,13 +3917,13 @@
     </row>
     <row r="10" ht="60" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>49</v>
@@ -3802,13 +3931,13 @@
     </row>
     <row r="11" ht="45" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>49</v>
@@ -3816,13 +3945,13 @@
     </row>
     <row r="12" ht="45" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>49</v>
@@ -3830,13 +3959,13 @@
     </row>
     <row r="13" ht="45" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
@@ -3844,13 +3973,13 @@
     </row>
     <row r="14" ht="30" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
@@ -3858,13 +3987,13 @@
     </row>
     <row r="15" ht="45" spans="1:4">
       <c r="A15" s="5" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>49</v>
@@ -3872,13 +4001,13 @@
     </row>
     <row r="16" ht="60" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>49</v>
@@ -3886,13 +4015,13 @@
     </row>
     <row r="17" ht="45" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
@@ -3900,13 +4029,13 @@
     </row>
     <row r="18" ht="30" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>49</v>
@@ -3914,13 +4043,13 @@
     </row>
     <row r="19" ht="30" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>49</v>
@@ -3928,13 +4057,13 @@
     </row>
     <row r="20" ht="45" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>49</v>
@@ -3942,13 +4071,13 @@
     </row>
     <row r="21" ht="45" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>49</v>
@@ -3956,13 +4085,13 @@
     </row>
     <row r="22" ht="30" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>49</v>
@@ -3970,13 +4099,13 @@
     </row>
     <row r="23" ht="30" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>49</v>
@@ -3984,13 +4113,13 @@
     </row>
     <row r="24" ht="30" spans="1:4">
       <c r="A24" s="5" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>49</v>
@@ -3998,13 +4127,13 @@
     </row>
     <row r="25" ht="30" spans="1:4">
       <c r="A25" s="5" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>49</v>
@@ -4012,13 +4141,13 @@
     </row>
     <row r="26" ht="30" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>49</v>
@@ -4026,13 +4155,13 @@
     </row>
     <row r="27" ht="45" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>49</v>
@@ -4040,13 +4169,13 @@
     </row>
     <row r="28" ht="30" spans="1:4">
       <c r="A28" s="5" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>49</v>
@@ -4054,13 +4183,13 @@
     </row>
     <row r="29" ht="30" spans="1:4">
       <c r="A29" s="5" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>49</v>
@@ -4068,13 +4197,13 @@
     </row>
     <row r="30" ht="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>49</v>
@@ -4082,13 +4211,13 @@
     </row>
     <row r="31" ht="30" spans="1:4">
       <c r="A31" s="5" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>49</v>
@@ -4096,13 +4225,13 @@
     </row>
     <row r="32" ht="30" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>49</v>
@@ -4152,13 +4281,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="95" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -4166,13 +4295,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="45" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -4180,13 +4309,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="93" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -4237,13 +4366,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -4251,13 +4380,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="33" customHeight="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -4265,13 +4394,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="34" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Product Strip Page and Email Notification functionailty modified
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -57,39 +57,39 @@
     <t>Cart page</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Suite1</t>
+  </si>
+  <si>
+    <t>Checkout Page</t>
+  </si>
+  <si>
+    <t>Suite2</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Suite3</t>
+  </si>
+  <si>
+    <t>Order Summary Page</t>
+  </si>
+  <si>
+    <t>Suite4</t>
+  </si>
+  <si>
+    <t>URL Tests</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Suite1</t>
-  </si>
-  <si>
-    <t>Checkout Page</t>
-  </si>
-  <si>
-    <t>Suite2</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Suite3</t>
-  </si>
-  <si>
-    <t>Order Summary Page</t>
-  </si>
-  <si>
-    <t>Suite4</t>
-  </si>
-  <si>
-    <t>URL Tests</t>
-  </si>
-  <si>
     <t>REST</t>
   </si>
   <si>
@@ -150,7 +150,7 @@
     <t>EMAIL ID</t>
   </si>
   <si>
-    <t>test@test.com, b@tx.com</t>
+    <t>sanyam.arora@testingxperts.com</t>
   </si>
   <si>
     <t>HTML Report</t>
@@ -995,14 +995,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1013,9 +1006,30 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1023,21 +1037,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1052,9 +1051,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1067,9 +1073,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1083,9 +1089,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1100,16 +1105,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1120,15 +1126,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1170,13 +1170,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,7 +1200,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1206,31 +1320,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1248,109 +1338,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1394,26 +1394,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1433,37 +1424,40 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1483,11 +1477,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1496,142 +1496,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1721,6 +1721,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="58" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2113,7 +2116,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2169,7 +2172,7 @@
       </c>
       <c r="E3" s="25">
         <f>IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:5">
@@ -2187,7 +2190,7 @@
       </c>
       <c r="E4" s="25">
         <f>IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:5">
@@ -2195,13 +2198,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="25">
         <f>IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
@@ -2210,16 +2213,16 @@
     </row>
     <row r="6" ht="15.75" spans="1:5">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="25">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
@@ -2228,10 +2231,10 @@
     </row>
     <row r="7" ht="15.75" spans="1:5">
       <c r="A7" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>19</v>
@@ -2241,14 +2244,14 @@
       </c>
       <c r="E7" s="25">
         <f>IF(B7="Y",COUNTIF(Suite5!B2:B51,"Y"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:5">
       <c r="A8" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="25" t="s">
@@ -2259,15 +2262,15 @@
       </c>
       <c r="E8" s="25">
         <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:5">
       <c r="A9" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>8</v>
+      <c r="B9" s="25" t="s">
+        <v>18</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>9</v>
@@ -2283,7 +2286,7 @@
       <c r="A10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
@@ -2300,7 +2303,7 @@
       <c r="A11" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -2313,23 +2316,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" ht="15.75" spans="1:5">
       <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" ht="15.75" spans="1:5">
       <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" ht="15.75" spans="1:5">
       <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -2388,7 +2391,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -2400,7 +2403,7 @@
       </c>
       <c r="B21" s="29">
         <f>SUM(E3:E15)</f>
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2433,7 +2436,7 @@
       <c r="A25" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="30" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="26"/>
@@ -2445,7 +2448,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -2456,7 +2459,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -2467,7 +2470,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -2489,19 +2492,22 @@
     </row>
     <row r="31" ht="15.75" spans="1:5">
       <c r="A31" s="27"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
     </row>
     <row r="32" ht="15.75" spans="1:5">
       <c r="A32" s="27"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1" display="sanyam.arora@testingxperts.com"/>
+  </hyperlinks>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
@@ -2542,7 +2548,7 @@
         <v>283</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>284</v>
@@ -2556,7 +2562,7 @@
         <v>285</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>286</v>
@@ -2570,7 +2576,7 @@
         <v>287</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>288</v>
@@ -2621,7 +2627,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>48</v>
@@ -2635,7 +2641,7 @@
         <v>50</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>51</v>
@@ -2649,7 +2655,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>53</v>
@@ -2663,7 +2669,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>55</v>
@@ -2677,7 +2683,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>57</v>
@@ -2691,7 +2697,7 @@
         <v>59</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>60</v>
@@ -2705,7 +2711,7 @@
         <v>61</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>62</v>
@@ -2719,7 +2725,7 @@
         <v>63</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>64</v>
@@ -2733,7 +2739,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>66</v>
@@ -2748,7 +2754,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>68</v>
@@ -2762,7 +2768,7 @@
         <v>69</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>70</v>
@@ -2776,7 +2782,7 @@
         <v>71</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>72</v>
@@ -2790,7 +2796,7 @@
         <v>73</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>74</v>
@@ -2804,7 +2810,7 @@
         <v>75</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>76</v>
@@ -2818,7 +2824,7 @@
         <v>77</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>78</v>
@@ -2832,7 +2838,7 @@
         <v>79</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>80</v>
@@ -2846,7 +2852,7 @@
         <v>81</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>82</v>
@@ -2894,7 +2900,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>84</v>
@@ -2905,7 +2911,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>86</v>
@@ -2916,7 +2922,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>88</v>
@@ -2927,7 +2933,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>90</v>
@@ -2938,7 +2944,7 @@
         <v>91</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>92</v>
@@ -2949,7 +2955,7 @@
         <v>93</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>94</v>
@@ -2960,7 +2966,7 @@
         <v>95</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>96</v>
@@ -2971,7 +2977,7 @@
         <v>97</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>98</v>
@@ -2982,7 +2988,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>100</v>
@@ -2993,7 +2999,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>102</v>
@@ -3004,7 +3010,7 @@
         <v>103</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>104</v>
@@ -3015,7 +3021,7 @@
         <v>105</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>104</v>
@@ -3026,7 +3032,7 @@
         <v>106</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>107</v>
@@ -3037,7 +3043,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>109</v>
@@ -3048,7 +3054,7 @@
         <v>110</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>111</v>
@@ -3059,7 +3065,7 @@
         <v>112</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>113</v>
@@ -3070,7 +3076,7 @@
         <v>114</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>115</v>
@@ -3081,7 +3087,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>117</v>
@@ -3092,7 +3098,7 @@
         <v>118</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>119</v>
@@ -3103,7 +3109,7 @@
         <v>120</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>121</v>
@@ -3114,7 +3120,7 @@
         <v>122</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>123</v>
@@ -3125,7 +3131,7 @@
         <v>124</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>125</v>
@@ -3136,7 +3142,7 @@
         <v>126</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>127</v>
@@ -3147,7 +3153,7 @@
         <v>128</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>129</v>
@@ -3158,7 +3164,7 @@
         <v>130</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>131</v>
@@ -3169,7 +3175,7 @@
         <v>132</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>133</v>
@@ -3180,7 +3186,7 @@
         <v>134</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>135</v>
@@ -3191,7 +3197,7 @@
         <v>136</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>137</v>
@@ -3202,7 +3208,7 @@
         <v>138</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>139</v>
@@ -3256,7 +3262,7 @@
         <v>140</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>141</v>
@@ -3270,7 +3276,7 @@
         <v>142</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>143</v>
@@ -3284,7 +3290,7 @@
         <v>144</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>145</v>
@@ -3298,7 +3304,7 @@
         <v>146</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>147</v>
@@ -3312,7 +3318,7 @@
         <v>148</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>149</v>
@@ -3326,7 +3332,7 @@
         <v>150</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>151</v>
@@ -3340,7 +3346,7 @@
         <v>152</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>153</v>
@@ -3354,7 +3360,7 @@
         <v>154</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>155</v>
@@ -3368,7 +3374,7 @@
         <v>156</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>157</v>
@@ -3382,7 +3388,7 @@
         <v>158</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>159</v>
@@ -3396,7 +3402,7 @@
         <v>160</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>161</v>
@@ -3410,7 +3416,7 @@
         <v>162</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>163</v>
@@ -3424,7 +3430,7 @@
         <v>164</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>165</v>
@@ -3438,7 +3444,7 @@
         <v>166</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>167</v>
@@ -3452,7 +3458,7 @@
         <v>168</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>169</v>
@@ -3466,7 +3472,7 @@
         <v>170</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>171</v>
@@ -3480,7 +3486,7 @@
         <v>172</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>173</v>
@@ -3494,7 +3500,7 @@
         <v>174</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>175</v>
@@ -3508,7 +3514,7 @@
         <v>176</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>177</v>
@@ -3522,7 +3528,7 @@
         <v>178</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>179</v>
@@ -3536,7 +3542,7 @@
         <v>180</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>181</v>
@@ -3550,7 +3556,7 @@
         <v>182</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>183</v>
@@ -3564,7 +3570,7 @@
         <v>184</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>185</v>
@@ -3578,7 +3584,7 @@
         <v>186</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>187</v>
@@ -3592,7 +3598,7 @@
         <v>189</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>190</v>
@@ -3645,7 +3651,7 @@
         <v>191</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>192</v>
@@ -3659,7 +3665,7 @@
         <v>193</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>194</v>
@@ -3673,7 +3679,7 @@
         <v>195</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>196</v>
@@ -3687,7 +3693,7 @@
         <v>197</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>198</v>
@@ -3701,7 +3707,7 @@
         <v>199</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>200</v>
@@ -3715,7 +3721,7 @@
         <v>201</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>202</v>
@@ -3729,7 +3735,7 @@
         <v>203</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>204</v>
@@ -3743,7 +3749,7 @@
         <v>205</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>206</v>
@@ -3798,7 +3804,7 @@
         <v>207</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>208</v>
@@ -3853,7 +3859,7 @@
         <v>209</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>210</v>
@@ -3867,7 +3873,7 @@
         <v>211</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>212</v>
@@ -3881,7 +3887,7 @@
         <v>213</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>214</v>
@@ -3895,7 +3901,7 @@
         <v>215</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>216</v>
@@ -3909,7 +3915,7 @@
         <v>217</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>218</v>
@@ -3923,7 +3929,7 @@
         <v>219</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>220</v>
@@ -3937,7 +3943,7 @@
         <v>221</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>222</v>
@@ -3951,7 +3957,7 @@
         <v>223</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>224</v>
@@ -3965,7 +3971,7 @@
         <v>225</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>226</v>
@@ -3979,7 +3985,7 @@
         <v>227</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>228</v>
@@ -3993,7 +3999,7 @@
         <v>229</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>230</v>
@@ -4007,7 +4013,7 @@
         <v>231</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>232</v>
@@ -4021,7 +4027,7 @@
         <v>233</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>234</v>
@@ -4035,7 +4041,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>236</v>
@@ -4049,7 +4055,7 @@
         <v>237</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>238</v>
@@ -4063,7 +4069,7 @@
         <v>239</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>240</v>
@@ -4077,7 +4083,7 @@
         <v>241</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>242</v>
@@ -4091,7 +4097,7 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>244</v>
@@ -4105,7 +4111,7 @@
         <v>245</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>246</v>
@@ -4119,7 +4125,7 @@
         <v>247</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>248</v>
@@ -4133,7 +4139,7 @@
         <v>249</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>250</v>
@@ -4147,7 +4153,7 @@
         <v>251</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>252</v>
@@ -4161,7 +4167,7 @@
         <v>253</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>254</v>
@@ -4175,7 +4181,7 @@
         <v>255</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>256</v>
@@ -4189,7 +4195,7 @@
         <v>257</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>258</v>
@@ -4203,7 +4209,7 @@
         <v>259</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>260</v>
@@ -4217,7 +4223,7 @@
         <v>261</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>262</v>
@@ -4231,7 +4237,7 @@
         <v>263</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>264</v>
@@ -4245,7 +4251,7 @@
         <v>265</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>266</v>
@@ -4259,7 +4265,7 @@
         <v>267</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>268</v>
@@ -4273,7 +4279,7 @@
         <v>269</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>270</v>
@@ -4329,7 +4335,7 @@
         <v>271</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>272</v>
@@ -4343,7 +4349,7 @@
         <v>273</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>274</v>
@@ -4357,7 +4363,7 @@
         <v>275</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>276</v>
@@ -4414,7 +4420,7 @@
         <v>277</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>278</v>
@@ -4428,7 +4434,7 @@
         <v>279</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>280</v>
@@ -4442,7 +4448,7 @@
         <v>281</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>282</v>

</xml_diff>

<commit_message>
Send mail code changed
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="987"/>
+    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="987" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -58,37 +58,37 @@
     <t>Cart page</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Suite1</t>
+  </si>
+  <si>
+    <t>Checkout Page</t>
+  </si>
+  <si>
+    <t>Suite2</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Suite3</t>
+  </si>
+  <si>
+    <t>Order Summary Page</t>
+  </si>
+  <si>
+    <t>Suite4</t>
+  </si>
+  <si>
+    <t>URL Tests</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Suite1</t>
-  </si>
-  <si>
-    <t>Checkout Page</t>
-  </si>
-  <si>
-    <t>Suite2</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Suite3</t>
-  </si>
-  <si>
-    <t>Order Summary Page</t>
-  </si>
-  <si>
-    <t>Suite4</t>
-  </si>
-  <si>
-    <t>URL Tests</t>
   </si>
   <si>
     <t>REST</t>
@@ -1053,6 +1053,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1080,6 +1087,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1099,6 +1113,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1144,28 +1165,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1179,6 +1179,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1186,13 +1193,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1228,24 +1228,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1264,25 +1246,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,7 +1276,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1331,6 +1367,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1355,60 +1409,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1554,138 +1554,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2173,8 +2173,8 @@
   <sheetPr/>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="E3" s="25">
         <f>IF(B3="Y",COUNTIF(Suite1!B2:B49,"Y"),0)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:5">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="E4" s="25">
         <f>IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:5">
@@ -2256,13 +2256,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="25">
         <f>IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
@@ -2271,16 +2271,16 @@
     </row>
     <row r="6" ht="15.75" spans="1:5">
       <c r="A6" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="25">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
@@ -2289,10 +2289,10 @@
     </row>
     <row r="7" ht="15.75" spans="1:5">
       <c r="A7" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>19</v>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="E7" s="25">
         <f>IF(B7="Y",COUNTIF(Suite5!B2:B51,"Y"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:5">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="E8" s="25">
         <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:5">
@@ -2362,7 +2362,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>9</v>
@@ -2379,7 +2379,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>9</v>
@@ -2457,7 +2457,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B21" s="29">
         <f>SUM(E3:E15)</f>
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2514,7 +2514,7 @@
         <v>42</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -2525,7 +2525,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -2536,7 +2536,7 @@
         <v>44</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -2585,8 +2585,8 @@
   <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -2614,7 +2614,7 @@
         <v>282</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>283</v>
@@ -2692,7 +2692,7 @@
         <v>288</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>289</v>
@@ -2706,7 +2706,7 @@
         <v>290</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>291</v>
@@ -2720,7 +2720,7 @@
         <v>292</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>293</v>
@@ -2734,7 +2734,7 @@
         <v>294</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>295</v>
@@ -2748,7 +2748,7 @@
         <v>296</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>297</v>
@@ -2762,7 +2762,7 @@
         <v>298</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>299</v>
@@ -2776,7 +2776,7 @@
         <v>300</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>301</v>
@@ -2790,7 +2790,7 @@
         <v>302</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>303</v>
@@ -2804,7 +2804,7 @@
         <v>304</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>305</v>
@@ -2818,7 +2818,7 @@
         <v>306</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>307</v>
@@ -2857,7 +2857,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="$A6:$XFD6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -3098,7 +3098,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>81</v>
@@ -3116,7 +3116,7 @@
   <sheetPr/>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3146,7 +3146,7 @@
         <v>82</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>83</v>
@@ -3366,7 +3366,7 @@
         <v>121</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>122</v>
@@ -3454,7 +3454,7 @@
         <v>137</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>138</v>
@@ -3508,7 +3508,7 @@
         <v>139</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>140</v>
@@ -3522,7 +3522,7 @@
         <v>141</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>142</v>
@@ -3536,7 +3536,7 @@
         <v>143</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>144</v>
@@ -3550,7 +3550,7 @@
         <v>145</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>146</v>
@@ -3564,7 +3564,7 @@
         <v>147</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>148</v>
@@ -3578,7 +3578,7 @@
         <v>149</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>150</v>
@@ -3592,7 +3592,7 @@
         <v>151</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>152</v>
@@ -3606,7 +3606,7 @@
         <v>153</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>154</v>
@@ -3620,7 +3620,7 @@
         <v>155</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>156</v>
@@ -3634,7 +3634,7 @@
         <v>157</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>158</v>
@@ -3648,7 +3648,7 @@
         <v>159</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>160</v>
@@ -3662,7 +3662,7 @@
         <v>161</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>162</v>
@@ -3676,7 +3676,7 @@
         <v>163</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>164</v>
@@ -3690,7 +3690,7 @@
         <v>165</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>166</v>
@@ -3704,7 +3704,7 @@
         <v>167</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>168</v>
@@ -3718,7 +3718,7 @@
         <v>169</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>170</v>
@@ -3732,7 +3732,7 @@
         <v>171</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>172</v>
@@ -3746,7 +3746,7 @@
         <v>173</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>174</v>
@@ -3760,7 +3760,7 @@
         <v>175</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>176</v>
@@ -3774,7 +3774,7 @@
         <v>177</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>178</v>
@@ -3788,7 +3788,7 @@
         <v>179</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>180</v>
@@ -3802,7 +3802,7 @@
         <v>181</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>182</v>
@@ -3816,7 +3816,7 @@
         <v>183</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>184</v>
@@ -3830,7 +3830,7 @@
         <v>185</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>186</v>
@@ -3844,7 +3844,7 @@
         <v>188</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>189</v>
@@ -3897,7 +3897,7 @@
         <v>190</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>191</v>
@@ -3911,7 +3911,7 @@
         <v>192</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>193</v>
@@ -3925,7 +3925,7 @@
         <v>194</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>195</v>
@@ -3939,7 +3939,7 @@
         <v>196</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>197</v>
@@ -3953,7 +3953,7 @@
         <v>198</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>199</v>
@@ -3967,7 +3967,7 @@
         <v>200</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>201</v>
@@ -3981,7 +3981,7 @@
         <v>202</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>203</v>
@@ -3995,7 +3995,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>205</v>
@@ -4050,7 +4050,7 @@
         <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>207</v>
@@ -4074,7 +4074,7 @@
   <sheetPr/>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
@@ -4105,7 +4105,7 @@
         <v>208</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>209</v>
@@ -4119,7 +4119,7 @@
         <v>210</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>211</v>
@@ -4133,7 +4133,7 @@
         <v>212</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>213</v>
@@ -4147,7 +4147,7 @@
         <v>214</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>215</v>
@@ -4161,7 +4161,7 @@
         <v>216</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>217</v>
@@ -4175,7 +4175,7 @@
         <v>218</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>219</v>
@@ -4189,7 +4189,7 @@
         <v>220</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>221</v>
@@ -4203,7 +4203,7 @@
         <v>222</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>223</v>
@@ -4217,7 +4217,7 @@
         <v>224</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>225</v>
@@ -4231,7 +4231,7 @@
         <v>226</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>227</v>
@@ -4245,7 +4245,7 @@
         <v>228</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>229</v>
@@ -4259,7 +4259,7 @@
         <v>230</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>231</v>
@@ -4273,7 +4273,7 @@
         <v>232</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>233</v>
@@ -4287,7 +4287,7 @@
         <v>234</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>235</v>
@@ -4301,7 +4301,7 @@
         <v>236</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>237</v>
@@ -4315,7 +4315,7 @@
         <v>238</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>239</v>
@@ -4329,7 +4329,7 @@
         <v>240</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>241</v>
@@ -4343,7 +4343,7 @@
         <v>242</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>243</v>
@@ -4357,7 +4357,7 @@
         <v>244</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>245</v>
@@ -4371,7 +4371,7 @@
         <v>246</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>247</v>
@@ -4385,7 +4385,7 @@
         <v>248</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>249</v>
@@ -4399,7 +4399,7 @@
         <v>250</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>251</v>
@@ -4413,7 +4413,7 @@
         <v>252</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>253</v>
@@ -4427,7 +4427,7 @@
         <v>254</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>255</v>
@@ -4441,7 +4441,7 @@
         <v>256</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>257</v>
@@ -4455,7 +4455,7 @@
         <v>258</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>259</v>
@@ -4469,7 +4469,7 @@
         <v>260</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>261</v>
@@ -4483,7 +4483,7 @@
         <v>262</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>263</v>
@@ -4497,7 +4497,7 @@
         <v>264</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>265</v>
@@ -4511,7 +4511,7 @@
         <v>266</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>267</v>
@@ -4525,7 +4525,7 @@
         <v>268</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>269</v>
@@ -4553,7 +4553,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -4581,7 +4581,7 @@
         <v>270</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>271</v>
@@ -4636,7 +4636,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -4666,7 +4666,7 @@
         <v>276</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>277</v>

</xml_diff>

<commit_message>
Order Summary tests added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -1173,6 +1173,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1180,13 +1187,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1222,6 +1222,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1229,6 +1235,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1246,7 +1258,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1276,30 +1300,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1318,13 +1318,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1342,19 +1354,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1366,13 +1372,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1384,25 +1396,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1548,7 +1548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1556,130 +1556,130 @@
     <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2168,7 +2168,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2265,7 +2265,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>9</v>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="E6" s="25">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:5">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B21" s="29">
         <f>SUM(E3:E15)</f>
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2794,7 +2794,7 @@
         <v>304</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>305</v>
@@ -4050,7 +4050,7 @@
   <sheetPr/>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sign Up Page Tests added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7770" tabRatio="987"/>
+    <workbookView windowWidth="20385" windowHeight="7770" tabRatio="987" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -971,7 +971,19 @@
     <t>Check whether a new user is able to Sign Up.</t>
   </si>
   <si>
-    <t>User should signup from HomePage.</t>
+    <t>IGP_TC_011</t>
+  </si>
+  <si>
+    <t>SignUp:User should signup from HomePage.</t>
+  </si>
+  <si>
+    <t>IGP_TC_012</t>
+  </si>
+  <si>
+    <t>SignUp:Duplicate Email Id/Number.</t>
+  </si>
+  <si>
+    <t>IGP_TC_013</t>
   </si>
 </sst>
 </file>
@@ -979,10 +991,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1050,6 +1062,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1057,8 +1074,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1071,36 +1097,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1115,6 +1113,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -1125,7 +1130,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1140,14 +1159,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1155,25 +1166,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1193,6 +1190,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1226,7 +1238,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1238,25 +1286,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1274,115 +1304,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1394,7 +1316,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1407,6 +1329,96 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1450,6 +1462,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1474,22 +1497,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1509,17 +1527,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1552,138 +1564,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2171,7 +2183,7 @@
   <sheetPr/>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B12"/>
     </sheetView>
   </sheetViews>
@@ -2849,13 +2861,13 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
@@ -2878,15 +2890,43 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="30" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="D2" s="5"/>
+        <v>307</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="30" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>